<commit_message>
bug reports added, cases modified
</commit_message>
<xml_diff>
--- a/Check.xlsx
+++ b/Check.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IdeaProjects\QAMID62-diplom-Shvets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A703101-1E74-452B-A111-B001475EEB69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12FBF0D-AF91-40ED-BD0A-46B7BD91AFF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2220" yWindow="1350" windowWidth="23190" windowHeight="13005" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Чек-лист" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
   <si>
     <t>Группа проверок/модуль</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Приоритет</t>
   </si>
   <si>
-    <t>Пройдено</t>
-  </si>
-  <si>
     <t>1. Установка, запуск, авторизация, удаление</t>
   </si>
   <si>
@@ -41,9 +38,6 @@
   </si>
   <si>
     <t>High</t>
-  </si>
-  <si>
-    <t>нет</t>
   </si>
   <si>
     <t>2. Корректный запуск (без зависаний и крэшей) приложения, отображение заставки</t>
@@ -157,11 +151,15 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="6">
@@ -532,10 +530,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -543,10 +541,9 @@
     <col min="1" max="1" width="28.28515625" customWidth="1"/>
     <col min="2" max="2" width="120.5703125" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -556,348 +553,264 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="12"/>
       <c r="B3" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
       <c r="B4" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="11"/>
       <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="B6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>13</v>
-      </c>
       <c r="C6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
       <c r="B7" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
       <c r="B8" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
       <c r="B9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="C10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
       <c r="B11" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="12"/>
       <c r="B12" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
       <c r="B14" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="14"/>
       <c r="B16" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="14"/>
       <c r="B17" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="14"/>
       <c r="B18" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="14"/>
       <c r="B19" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="15"/>
       <c r="B20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="9" t="s">
+      <c r="C21" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B22" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="C22" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
       <c r="B23" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="C24" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="11"/>
       <c r="B25" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A26" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="C26" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="12"/>
       <c r="B27" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
       <c r="B28" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>